<commit_message>
🚀 Campos de faltaban #95
</commit_message>
<xml_diff>
--- a/procesador/datos/Listado de proyectos - 60 años dpto antropología .xlsx
+++ b/procesador/datos/Listado de proyectos - 60 años dpto antropología .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/a_ulloag_uniandes_edu_co/Documents/60 años departamento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{102CE23C-DF61-40EB-ABFE-FC38ACB7F9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AF422EF-96D1-4D19-B738-4F9C427BD600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40460" yWindow="1220" windowWidth="36630" windowHeight="19120" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40460" yWindow="1220" windowWidth="36630" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proyectos" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="2896" r:id="rId15"/>
+    <pivotCache cacheId="6076" r:id="rId15"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2795,7 +2795,7 @@
     <t>GuiaBasica_Portada</t>
   </si>
   <si>
-    <t>GuiaBasica_Pdf</t>
+    <t>GuiaBasica_Pdf.pdf</t>
   </si>
   <si>
     <t>Plan Nacional de Rehabilitación</t>
@@ -14608,10 +14608,7 @@
     <t>Victoria Cunningham</t>
   </si>
   <si>
-    <t>Sector público
-Sector privado
-Academia
-Consultoría</t>
+    <t>Sector público;Sector privado;Academia;Consultoría;</t>
   </si>
   <si>
     <t>Valentina Correa</t>
@@ -14632,11 +14629,7 @@
     <t>Nicolás Aguilar-Forero</t>
   </si>
   <si>
-    <t>Sector público
-Sector privado
-Academia
-ONG
-Consultoría</t>
+    <t>Sector público;Sector privado;Academia;ONG;Consultoría</t>
   </si>
   <si>
     <t>Juana Ochoa Almanza</t>
@@ -14653,9 +14646,7 @@
     <t>Nelson Javier Vera Guerrero</t>
   </si>
   <si>
-    <t>Sector público
-Sector privado
-Academia</t>
+    <t>Sector público;Sector privado;Academia;</t>
   </si>
   <si>
     <t>Mario Andrés Rodríguez Larrota</t>
@@ -14739,8 +14730,7 @@
     <t>Esteban Narváez Polo</t>
   </si>
   <si>
-    <t>Sector público
-Academia</t>
+    <t>Sector público;Academia</t>
   </si>
   <si>
     <t>País: 
@@ -20209,7 +20199,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4570351-E376-4474-B0C8-4F00FB638DE4}" name="Tabla dinámica1" cacheId="2896" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4570351-E376-4474-B0C8-4F00FB638DE4}" name="Tabla dinámica1" cacheId="6076" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A2:B37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
@@ -20786,9 +20776,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X152"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="7" topLeftCell="R133" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A143" sqref="A143:W143"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane xSplit="7" topLeftCell="T122" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W129" sqref="W129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -31164,14 +31154,14 @@
       <c r="S150" s="78" t="s">
         <v>929</v>
       </c>
-      <c r="T150" s="67" t="s">
-        <v>30</v>
-      </c>
-      <c r="U150" s="55" t="s">
+      <c r="T150" s="55" t="s">
         <v>930</v>
       </c>
-      <c r="V150" s="67" t="s">
+      <c r="U150" s="67" t="s">
         <v>931</v>
+      </c>
+      <c r="V150" s="55" t="s">
+        <v>30</v>
       </c>
       <c r="W150" s="67" t="s">
         <v>30</v>
@@ -31302,7 +31292,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:O1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:XFD3 N11:Q11 S11:T11 M19:M20 O19:T20 M31:S31 M32:N32 P32:T32 Q39:T39 M40:T40 L46 L56 L67 L86:L87 L97 K98:L98 P82:Q83 M82:O84 Q84 M17:T18 S113:T113 O12:T16 N81:Q81 M85:Q86 S81:T86 T126 M4:T8 L103:XFD103 L127:T128 L126:R126 I129:O129 Q129:XFD129 I130:XFD130 Q133:R133 I133:O133 S131:XFD134 I131:R132 I135:XFD136 G68 I67:J67 G85:L85 A109:C128 L109:T111 U108:XFD128 S108:T108 P108:Q108 E99:L99 H45:L45 H46:J46 H44:K44 H47:L48 E49:L54 H55:L55 H56:J56 E60 E61:F68 G86:J86 E95:L96 H87:J87 E85:F94 H88:L94 G87:G94 E108:G109 F129:G136 H115:T118 H119:K128 E113:Q113 E115:G128 E97:J98 M9:M16 M33:T38 M39:O39 N80:T80 M47 M49 M51 M59 M80:M81 M87:T101 L119:T125 J137:XFD137 M60:T79 E111:G112 E110 G110 L147:P147 J147:J148 A149:B150 I138:XFD139 P140:R141 I140:N140 M141:N141 H143:N143 M142:R142 S140:XFD142 A129:A148 B139:B148 G141:G148 I144:N146 J148:N148 E138:F146 P143:XFD148 F149:H150 J149:XFD150 N9:T10 M21:T30 C129:C151 I134:R134 A151:XFD151 A153:XFD1048576 A152:G152 P152:XFD152 I152:N152 E55:G58 D4:D150 U4:XFD101 B4:C108 H57:L58 M52:T58 E4:L39 E40:G48 H40:L43 E69:G71 I68:L71 E72:L84 I104:XFD104 I103:J103 I102:XFD102 I100:L101 E100:H104 E105:XFD107 I109:J111 I112:T112 I108:N108 H108:H112 E114:T114 I141:L142 H144:H148">
+  <conditionalFormatting sqref="A1:XFD3 N11:Q11 S11:T11 M19:M20 O19:T20 M31:S31 M32:N32 P32:T32 Q39:T39 M40:T40 L46 L56 L67 L86:L87 L97 K98:L98 P82:Q83 M82:O84 Q84 M17:T18 S113:T113 O12:T16 N81:Q81 M85:Q86 S81:T86 T126 M4:T8 L103:XFD103 L127:T128 L126:R126 I129:O129 Q129:XFD129 I130:XFD130 Q133:R133 I133:O133 S131:XFD134 I131:R132 I135:XFD136 G68 I67:J67 G85:L85 A109:C128 L109:T111 U108:XFD128 S108:T108 P108:Q108 E99:L99 H45:L45 H46:J46 H44:K44 H47:L48 E49:L54 H55:L55 H56:J56 E60 E61:F68 G86:J86 E95:L96 H87:J87 E85:F94 H88:L94 G87:G94 E108:G109 F129:G136 H115:T118 H119:K128 E113:Q113 E115:G128 E97:J98 M9:M16 M33:T38 M39:O39 N80:T80 M47 M49 M51 M59 M80:M81 M87:T101 L119:T125 J137:XFD137 M60:T79 E111:G112 E110 G110 L147:P147 J147:J148 A149:B150 I138:XFD139 P140:R141 I140:N140 M141:N141 H143:N143 M142:R142 S140:XFD142 A129:A148 B139:B148 G141:G148 I144:N146 J148:N148 E138:F146 P143:XFD148 F149:H150 N9:T10 M21:T30 C129:C151 I134:R134 A151:XFD151 A153:XFD1048576 A152:G152 P152:XFD152 I152:N152 E55:G58 D4:D150 U4:XFD101 B4:C108 H57:L58 M52:T58 E4:L39 E40:G48 H40:L43 E69:G71 I68:L71 E72:L84 I104:XFD104 I103:J103 I102:XFD102 I100:L101 E100:H104 E105:XFD107 I109:J111 I112:T112 I108:N108 H108:H112 E114:T114 I141:L142 H144:H148 J149:XFD149 W150:XFD150 J150:U150">
     <cfRule type="cellIs" dxfId="42" priority="17" operator="equal">
       <formula>"Sin Información"</formula>
     </cfRule>
@@ -31312,14 +31302,14 @@
       <formula>"Sin Información"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U152">
+  <conditionalFormatting sqref="U3:U149 U151:U152 T150">
     <cfRule type="containsText" dxfId="40" priority="15" operator="containsText" text=".">
-      <formula>NOT(ISERROR(SEARCH(".",U3)))</formula>
+      <formula>NOT(ISERROR(SEARCH(".",T3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:U152">
+  <conditionalFormatting sqref="U3:U149 U151:U152 T150">
     <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="_10">
-      <formula>NOT(ISERROR(SEARCH("_10",U3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("_10",T3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B129">
@@ -78655,8 +78645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCD70B0-A791-439F-BF2F-1756F6282BE8}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>